<commit_message>
Update Grid Independence Test.xlsx
</commit_message>
<xml_diff>
--- a/Grid Independence Test.xlsx
+++ b/Grid Independence Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Donov\Documents\Georgia Tech\Fall 2022\Heat Transfer - ME 3345\Project\Heat-Transfer-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D845FA6-83EB-4621-8CC3-E7A0B11CA45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC38A32A-6D2B-4F4D-8652-1C720AC1B5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4407A9D0-A05B-499B-BABE-E677F4E1D6FE}"/>
+    <workbookView xWindow="-54705" yWindow="1755" windowWidth="23625" windowHeight="12630" xr2:uid="{4407A9D0-A05B-499B-BABE-E677F4E1D6FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>